<commit_message>
Fix Recipent by data import via excel.
</commit_message>
<xml_diff>
--- a/app/excel/test_recipients.xlsx
+++ b/app/excel/test_recipients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT BLASTING\sistem-operasional-yayasan-ypik\app\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B646F83A-F6EC-4A16-92C8-25DDAFB24080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920568ED-1980-47E7-826C-A3E1550AA38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="9420" xr2:uid="{387EF976-B422-44A1-938F-1BDBC39E8DED}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">NO </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>WA</t>
   </si>
@@ -45,52 +42,34 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>0878-8837-0352</t>
-  </si>
-  <si>
-    <t>0819-1120-4834</t>
-  </si>
-  <si>
-    <t>0878-8888-7777</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
-    <t>test6@gmail.com</t>
-  </si>
-  <si>
-    <t>test7@gmail.com</t>
-  </si>
-  <si>
-    <t>test8@gmail.com</t>
-  </si>
-  <si>
-    <t>test9@gmail.com</t>
-  </si>
-  <si>
-    <t>test10@gmail.com</t>
-  </si>
-  <si>
-    <t>Christopherateraputra1@gmail.com</t>
-  </si>
-  <si>
-    <t>Filmoraxadobe151@gmail.com</t>
+    <t>ito</t>
+  </si>
+  <si>
+    <t>ellan</t>
+  </si>
+  <si>
+    <t>shine</t>
+  </si>
+  <si>
+    <t>0878-7777-6670</t>
+  </si>
+  <si>
+    <t>0819-1166-1139</t>
+  </si>
+  <si>
+    <t>0878-8877-0217</t>
+  </si>
+  <si>
+    <t>nama_siswa</t>
+  </si>
+  <si>
+    <t>Ayamm1111@gmail.com</t>
+  </si>
+  <si>
+    <t>Bebek111@gmail.com</t>
+  </si>
+  <si>
+    <t>Kucinh2112@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -159,12 +138,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,189 +468,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC120A2-D82B-41EE-A895-84FA68E4DA70}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="46.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>515415451</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4848787</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4489787231</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>24878451</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>445054</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>69558512</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>878787478</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7971544</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>784132161</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>77778549848</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6C4949F7-EA84-4289-A981-B1851D0259B2}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{1309D0D5-B8CF-4714-AE0C-8DAC7D229688}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{1282A500-3ABA-4904-9D92-8363CDEEC356}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{3DD02537-8B2B-401A-A482-D7E63B9CD9A5}"/>
-    <hyperlink ref="C6:C14" r:id="rId5" display="test1@gmail.com" xr:uid="{DEEE5363-FE10-4EFF-9771-425589FC841E}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{7C09FE8E-56D5-4509-B7D1-0F537AD8FA0C}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{73857C57-47CB-46B8-89C7-D8C524AC9057}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{C9B1FE7F-CCAE-4877-B455-7BDAE1A34ED5}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{91BF4314-563A-4EDC-B5B4-FD48D8FD15FC}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{76551826-4790-4D0E-AC79-08B6C79A96C4}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{4788F8DF-175E-49F6-8813-55A404844F38}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{6017676F-0EB1-4D57-9A7A-402294CF2E16}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{3422EC86-9221-4311-ABB7-63739D824CE9}"/>
-    <hyperlink ref="C14" r:id="rId14" xr:uid="{827FA4CB-960A-4560-BEA7-CCE3B7241A22}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{C8E79C64-BD60-4291-A939-ADB484E07AA6}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F2C27D14-28EA-44B1-B3DD-7306C16128FB}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{05A086CB-7361-431E-8ECA-3122A0158F1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor web.php and add blast template.
</commit_message>
<xml_diff>
--- a/app/excel/test_recipients.xlsx
+++ b/app/excel/test_recipients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT BLASTING\sistem-operasional-yayasan-ypik\app\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920568ED-1980-47E7-826C-A3E1550AA38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDB59028-F689-4AEB-94C5-C47298DC6808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="9420" xr2:uid="{387EF976-B422-44A1-938F-1BDBC39E8DED}"/>
+    <workbookView xWindow="528" yWindow="2364" windowWidth="22596" windowHeight="6000" xr2:uid="{387EF976-B422-44A1-938F-1BDBC39E8DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>WA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>ito</t>
-  </si>
-  <si>
-    <t>ellan</t>
-  </si>
-  <si>
-    <t>shine</t>
-  </si>
-  <si>
     <t>0878-7777-6670</t>
   </si>
   <si>
@@ -60,9 +48,6 @@
     <t>0878-8877-0217</t>
   </si>
   <si>
-    <t>nama_siswa</t>
-  </si>
-  <si>
     <t>Ayamm1111@gmail.com</t>
   </si>
   <si>
@@ -70,6 +55,51 @@
   </si>
   <si>
     <t>Kucinh2112@gmail.com</t>
+  </si>
+  <si>
+    <t>nama siswa</t>
+  </si>
+  <si>
+    <t>Christo</t>
+  </si>
+  <si>
+    <t>Audy</t>
+  </si>
+  <si>
+    <t>Bowo</t>
+  </si>
+  <si>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>7A - IPA</t>
+  </si>
+  <si>
+    <t>10 -IPA</t>
+  </si>
+  <si>
+    <t>9B -IPS</t>
+  </si>
+  <si>
+    <t>Nama Wali</t>
+  </si>
+  <si>
+    <t>Bambang</t>
+  </si>
+  <si>
+    <t>Bayu</t>
+  </si>
+  <si>
+    <t>Santo</t>
+  </si>
+  <si>
+    <t>WhasApp</t>
+  </si>
+  <si>
+    <t>Catatan (Optional)</t>
+  </si>
+  <si>
+    <t>baik</t>
   </si>
 </sst>
 </file>
@@ -138,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,12 +176,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -468,119 +503,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC120A2-D82B-41EE-A895-84FA68E4DA70}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="C1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" customWidth="1"/>
+    <col min="3" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="46.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C8E79C64-BD60-4291-A939-ADB484E07AA6}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{F2C27D14-28EA-44B1-B3DD-7306C16128FB}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{05A086CB-7361-431E-8ECA-3122A0158F1E}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{C8E79C64-BD60-4291-A939-ADB484E07AA6}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{F2C27D14-28EA-44B1-B3DD-7306C16128FB}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{05A086CB-7361-431E-8ECA-3122A0158F1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>